<commit_message>
Add CargadorManzanas y visualizacion manzanas
</commit_message>
<xml_diff>
--- a/src/listas_de_manzanas/manzanasPrueba.xlsx
+++ b/src/listas_de_manzanas/manzanasPrueba.xlsx
@@ -19,15 +19,54 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
   <si>
     <t>Nro manzana</t>
   </si>
   <si>
-    <t>Coord X</t>
-  </si>
-  <si>
-    <t>Coord Y</t>
+    <t>Nro manzanas vecinas</t>
+  </si>
+  <si>
+    <t>Coordenadas</t>
+  </si>
+  <si>
+    <t>-34.51909573235544, -58.71988115476912</t>
+  </si>
+  <si>
+    <t>-34.52637948225431, -58.71009645709745</t>
+  </si>
+  <si>
+    <t>-34.528005863683184, -58.731039143342066</t>
+  </si>
+  <si>
+    <t>-34.54045016573941, -58.72511682633027</t>
+  </si>
+  <si>
+    <t>-34.54589396298188, -58.715589620702595</t>
+  </si>
+  <si>
+    <t>-34.53599588498832, -58.69670687080991</t>
+  </si>
+  <si>
+    <t>-34.553275292650206, -58.719442876513725</t>
+  </si>
+  <si>
+    <t>-34.56213183370967, -58.70717317543131</t>
+  </si>
+  <si>
+    <t>-34.5586715072938, -58.691521521470904</t>
+  </si>
+  <si>
+    <t>2,4,6</t>
+  </si>
+  <si>
+    <t>3,5,7</t>
+  </si>
+  <si>
+    <t>1,4,8</t>
+  </si>
+  <si>
+    <t>4,6,8</t>
   </si>
 </sst>
 </file>
@@ -63,8 +102,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -345,15 +385,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C9"/>
+  <dimension ref="A1:C10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+      <selection activeCell="B2" sqref="B2:C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="18" customWidth="1"/>
+    <col min="2" max="2" width="40.42578125" customWidth="1"/>
+    <col min="3" max="3" width="18" customWidth="1"/>
+    <col min="4" max="4" width="25.140625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
@@ -361,53 +404,113 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" t="s">
         <v>1</v>
-      </c>
-      <c r="C1" t="s">
-        <v>2</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>0</v>
       </c>
+      <c r="B2" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C2" s="1">
+        <v>2.1</v>
+      </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>1</v>
       </c>
+      <c r="B3" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C3" s="1">
+        <v>0.5</v>
+      </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>2</v>
       </c>
+      <c r="B4" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C4" s="1">
+        <v>0.3</v>
+      </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>3</v>
       </c>
+      <c r="B5" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>12</v>
+      </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>4</v>
       </c>
+      <c r="B6" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>5</v>
       </c>
+      <c r="B7" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>14</v>
+      </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>6</v>
       </c>
+      <c r="B8" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C8" s="1">
+        <v>3.7</v>
+      </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>7</v>
       </c>
+      <c r="B9" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>8</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C10" s="1">
+        <v>5.7</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="360" verticalDpi="360" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>